<commit_message>
Challenge 267,268 has been added.
</commit_message>
<xml_diff>
--- a/Excel Files/Excel Challenges/Challenge 267 - Highest Percentage of Bronze Medals.xlsx
+++ b/Excel Files/Excel Challenges/Challenge 267 - Highest Percentage of Bronze Medals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\Excel-BI-Python\Excel Files\Excel Challenges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D9B805D-574B-4EE8-96BF-DFD21F6BC321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F71EF00-0317-469B-9C7D-E8C87A3DC735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="34580" windowHeight="13980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -205,10 +205,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="distributed"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -789,6 +789,9 @@
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
@@ -834,11 +837,11 @@
         <v>3</v>
       </c>
       <c r="E1" s="2"/>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
@@ -864,7 +867,7 @@
         <v>7</v>
       </c>
       <c r="N2" s="6"/>
-      <c r="O2" s="10" cm="1">
+      <c r="O2" s="9" cm="1">
         <f t="array" ref="O2:Q5">_xlfn.LET(_xlpm.Data, A1:D10, _xlpm.OnlyData, _xlfn.DROP(_xlpm.Data, 1, 1), _xlpm.SumByRow, _xlfn.BYROW(_xlpm.OnlyData, _xlfn.LAMBDA(_xlpm.r, SUM(_xlpm.r))), _xlpm.BronzeData, _xlfn.CHOOSECOLS(_xlpm.OnlyData, _xlfn.XMATCH("Bronze", _xlfn.TAKE(_xlpm.Data, 1), 0) - 1), _xlpm.Percentage, (_xlpm.BronzeData / _xlpm.SumByRow) * 100, _xlpm.OnlyWholePart, ROUND(_xlpm.Percentage, 0), _xlpm.OnlyCountry, _xlfn.TAKE(_xlfn.DROP(_xlpm.Data, 1), , 1), _xlpm.Sorted, _xlfn.SORTBY(_xlfn.HSTACK(_xlpm.OnlyCountry, _xlpm.Percentage, _xlpm.OnlyWholePart), _xlpm.OnlyWholePart, -1), _xlpm.Rank, _xlfn.XMATCH(_xlfn.TAKE(_xlpm.Sorted, , -1), _xlfn.TAKE(_xlpm.Sorted, , -1), 0), _xlpm.Result, _xlfn._xlws.SORT(_xlfn._xlws.FILTER(_xlfn.HSTACK(_xlpm.Rank, _xlfn.DROP(_xlpm.Sorted, , -1)), _xlpm.Rank &lt;= 3), 2), _xlpm.Result)</f>
         <v>1</v>
       </c>

</xml_diff>